<commit_message>
12.26 figure init HOME
</commit_message>
<xml_diff>
--- a/astro/threshold00167_FFN/FFN.xlsx
+++ b/astro/threshold00167_FFN/FFN.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\astro\threshold00167_FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AF98C6-6C5D-4902-8AFA-4C0F73A53E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AC1573-0530-43DE-A9FD-303886CB2DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8544" yWindow="2832" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-492" yWindow="7356" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -436,7 +437,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>